<commit_message>
2012-9-26 Sashimi Modify some scripts.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST483_SelectOneOrMoreThanOneDeviceParameters.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST483_SelectOneOrMoreThanOneDeviceParameters.xlsx
@@ -1243,7 +1243,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7701" uniqueCount="862">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7711" uniqueCount="864">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3874,6 +3874,14 @@
   </si>
   <si>
     <t>$GXT_0$</t>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pause</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -4094,7 +4102,35 @@
     <cellStyle name="常规 2" xfId="1"/>
     <cellStyle name="超链接" xfId="2" builtinId="8"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4399,10 +4435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O64"/>
+  <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4609,7 +4645,7 @@
         <v>771</v>
       </c>
       <c r="B7" s="4">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C7" s="5">
         <v>6</v>
@@ -4640,34 +4676,24 @@
         <v>7</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>793</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>576</v>
+        <v>787</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>582</v>
-      </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="s">
-        <v>794</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>860</v>
-      </c>
-      <c r="J8" s="5" t="s">
-        <v>861</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>797</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>778</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>795</v>
-      </c>
-      <c r="N8" s="7"/>
+        <v>20</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="2"/>
     </row>
     <row r="9" spans="1:15">
@@ -4681,22 +4707,24 @@
         <v>8</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>843</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>844</v>
-      </c>
-      <c r="F9" s="5">
-        <v>2</v>
-      </c>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+        <v>787</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="11"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
       <c r="M9" s="5"/>
-      <c r="N9" s="7"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="2"/>
     </row>
     <row r="10" spans="1:15">
@@ -4706,24 +4734,22 @@
         <v>9</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>845</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10" s="5"/>
+        <v>862</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>863</v>
+      </c>
+      <c r="F10" s="11">
+        <v>2</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="11"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
       <c r="M10" s="5"/>
-      <c r="N10" s="7"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="2"/>
     </row>
     <row r="11" spans="1:15">
@@ -4735,23 +4761,33 @@
         <v>10</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>845</v>
+        <v>793</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>19</v>
+        <v>576</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>846</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>847</v>
-      </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
-      <c r="M11" s="5"/>
+        <v>582</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5" t="s">
+        <v>794</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>860</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>861</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>797</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>778</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>795</v>
+      </c>
       <c r="N11" s="7"/>
       <c r="O11" s="2"/>
     </row>
@@ -4764,20 +4800,16 @@
         <v>11</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>576</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>861</v>
-      </c>
+        <v>844</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -4798,10 +4830,10 @@
         <v>845</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>576</v>
+        <v>19</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>175</v>
+        <v>22</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>2</v>
@@ -4827,13 +4859,13 @@
         <v>845</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>518</v>
+        <v>19</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>525</v>
+        <v>846</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>2</v>
+        <v>847</v>
       </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
@@ -4856,15 +4888,17 @@
         <v>845</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>376</v>
+        <v>577</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15" s="5"/>
+        <v>56</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>861</v>
+      </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
@@ -4885,10 +4919,10 @@
         <v>845</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>17</v>
+        <v>175</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>2</v>
@@ -4917,7 +4951,7 @@
         <v>518</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>17</v>
+        <v>525</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>2</v>
@@ -4943,10 +4977,10 @@
         <v>845</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>95</v>
+        <v>376</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>2</v>
@@ -4960,7 +4994,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="15">
+    <row r="19" spans="1:15">
       <c r="A19" s="3" t="s">
         <v>783</v>
       </c>
@@ -4970,12 +5004,18 @@
       <c r="C19" s="5">
         <v>18</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>836</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
+      <c r="D19" s="8" t="s">
+        <v>845</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>574</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>2</v>
+      </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -4994,19 +5034,19 @@
         <v>19</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>19</v>
+        <v>845</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>518</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
       <c r="J20" s="5"/>
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
@@ -5023,23 +5063,19 @@
         <v>20</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>19</v>
+        <v>845</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>576</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H21" s="11">
-        <v>2</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>861</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H21" s="5"/>
+      <c r="I21" s="5"/>
       <c r="J21" s="5"/>
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
@@ -5047,23 +5083,17 @@
       <c r="N21" s="7"/>
       <c r="O21" s="2"/>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:15" ht="15">
       <c r="C22" s="5">
         <v>21</v>
       </c>
-      <c r="D22" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22" s="11"/>
+      <c r="D22" s="6" t="s">
+        <v>836</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
       <c r="K22" s="5"/>
@@ -5083,13 +5113,13 @@
         <v>19</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>109</v>
+        <v>26</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H23" s="11"/>
-      <c r="I23" s="5"/>
+      <c r="I23" s="11"/>
       <c r="J23" s="5"/>
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
@@ -5097,18 +5127,28 @@
       <c r="N23" s="7"/>
       <c r="O23" s="2"/>
     </row>
-    <row r="24" spans="1:15" ht="15">
+    <row r="24" spans="1:15">
       <c r="C24" s="5">
         <v>23</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>839</v>
-      </c>
-      <c r="E24" s="11"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="D24" s="8" t="s">
+        <v>787</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H24" s="11">
+        <v>2</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>861</v>
+      </c>
       <c r="J24" s="5"/>
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
@@ -5124,20 +5164,16 @@
         <v>787</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>574</v>
+        <v>19</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>575</v>
+        <v>102</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="H25" s="11">
-        <v>2</v>
-      </c>
-      <c r="I25" s="11">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="5"/>
       <c r="J25" s="5"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -5150,53 +5186,39 @@
         <v>25</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>798</v>
+        <v>787</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>574</v>
+        <v>19</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>575</v>
+        <v>109</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="H26" s="11">
-        <v>3</v>
-      </c>
-      <c r="I26" s="11">
-        <v>1</v>
-      </c>
-      <c r="J26" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="5"/>
+      <c r="J26" s="5"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
       <c r="M26" s="5"/>
       <c r="N26" s="7"/>
       <c r="O26" s="2"/>
     </row>
-    <row r="27" spans="1:15">
+    <row r="27" spans="1:15" ht="15">
       <c r="C27" s="5">
         <v>26</v>
       </c>
-      <c r="D27" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>574</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>575</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="H27" s="11">
-        <v>4</v>
-      </c>
-      <c r="I27" s="11">
-        <v>1</v>
-      </c>
-      <c r="J27" s="11"/>
+      <c r="D27" s="6" t="s">
+        <v>839</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="5"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
       <c r="M27" s="5"/>
@@ -5220,7 +5242,7 @@
         <v>831</v>
       </c>
       <c r="H28" s="11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I28" s="11">
         <v>1</v>
@@ -5237,7 +5259,7 @@
         <v>28</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>787</v>
+        <v>798</v>
       </c>
       <c r="E29" s="11" t="s">
         <v>574</v>
@@ -5249,12 +5271,12 @@
         <v>831</v>
       </c>
       <c r="H29" s="11">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I29" s="11">
         <v>1</v>
       </c>
-      <c r="J29" s="5"/>
+      <c r="J29" s="11"/>
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
       <c r="M29" s="5"/>
@@ -5278,12 +5300,12 @@
         <v>831</v>
       </c>
       <c r="H30" s="11">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I30" s="11">
         <v>1</v>
       </c>
-      <c r="J30" s="5"/>
+      <c r="J30" s="11"/>
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
       <c r="M30" s="5"/>
@@ -5307,7 +5329,7 @@
         <v>831</v>
       </c>
       <c r="H31" s="11">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I31" s="11">
         <v>1</v>
@@ -5336,7 +5358,7 @@
         <v>831</v>
       </c>
       <c r="H32" s="11">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="I32" s="11">
         <v>1</v>
@@ -5355,16 +5377,20 @@
         <v>787</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>857</v>
+        <v>574</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>17</v>
+        <v>575</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
+        <v>831</v>
+      </c>
+      <c r="H33" s="11">
+        <v>7</v>
+      </c>
+      <c r="I33" s="11">
+        <v>1</v>
+      </c>
       <c r="J33" s="5"/>
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
@@ -5379,16 +5405,20 @@
         <v>787</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>857</v>
+        <v>574</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>17</v>
+        <v>575</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
+        <v>831</v>
+      </c>
+      <c r="H34" s="11">
+        <v>8</v>
+      </c>
+      <c r="I34" s="11">
+        <v>1</v>
+      </c>
       <c r="J34" s="5"/>
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
@@ -5406,20 +5436,18 @@
         <v>574</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>331</v>
+        <v>575</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H35" s="11" t="s">
-        <v>852</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>853</v>
-      </c>
-      <c r="J35" s="5">
-        <v>30</v>
-      </c>
+        <v>831</v>
+      </c>
+      <c r="H35" s="11">
+        <v>9</v>
+      </c>
+      <c r="I35" s="11">
+        <v>1</v>
+      </c>
+      <c r="J35" s="5"/>
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
       <c r="M35" s="5"/>
@@ -5433,17 +5461,15 @@
         <v>787</v>
       </c>
       <c r="E36" s="11" t="s">
-        <v>574</v>
+        <v>857</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>331</v>
+        <v>17</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H36" s="11" t="s">
-        <v>854</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="H36" s="11"/>
       <c r="I36" s="11"/>
       <c r="J36" s="5"/>
       <c r="K36" s="5"/>
@@ -5459,17 +5485,15 @@
         <v>787</v>
       </c>
       <c r="E37" s="11" t="s">
-        <v>574</v>
+        <v>857</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>331</v>
+        <v>17</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H37" s="11" t="s">
-        <v>855</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H37" s="11"/>
       <c r="I37" s="11"/>
       <c r="J37" s="5"/>
       <c r="K37" s="5"/>
@@ -5488,14 +5512,20 @@
         <v>574</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>852</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="J38" s="5">
+        <v>30</v>
+      </c>
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
       <c r="M38" s="5"/>
@@ -5515,17 +5545,13 @@
         <v>331</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>851</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>853</v>
-      </c>
-      <c r="J39" s="5">
-        <v>10080</v>
-      </c>
+        <v>854</v>
+      </c>
+      <c r="I39" s="11"/>
+      <c r="J39" s="5"/>
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
       <c r="M39" s="5"/>
@@ -5548,7 +5574,7 @@
         <v>4</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="I40" s="11"/>
       <c r="J40" s="5"/>
@@ -5568,14 +5594,12 @@
         <v>574</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>856</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H41" s="11"/>
       <c r="I41" s="11"/>
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
@@ -5594,14 +5618,20 @@
         <v>574</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>847</v>
-      </c>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H42" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="J42" s="5">
+        <v>10080</v>
+      </c>
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
       <c r="M42" s="5"/>
@@ -5621,17 +5651,13 @@
         <v>331</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H43" s="11" t="s">
-        <v>851</v>
-      </c>
-      <c r="I43" s="11" t="s">
-        <v>853</v>
-      </c>
-      <c r="J43" s="5">
-        <v>1</v>
-      </c>
+        <v>854</v>
+      </c>
+      <c r="I43" s="11"/>
+      <c r="J43" s="5"/>
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
       <c r="M43" s="5"/>
@@ -5648,12 +5674,14 @@
         <v>574</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>17</v>
+        <v>331</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="H44" s="11" t="s">
+        <v>856</v>
+      </c>
       <c r="I44" s="11"/>
       <c r="J44" s="5"/>
       <c r="K44" s="5"/>
@@ -5666,15 +5694,17 @@
         <v>44</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>843</v>
+        <v>787</v>
       </c>
       <c r="E45" s="11" t="s">
-        <v>844</v>
-      </c>
-      <c r="F45" s="5">
-        <v>2</v>
-      </c>
-      <c r="G45" s="5"/>
+        <v>574</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>847</v>
+      </c>
       <c r="H45" s="11"/>
       <c r="I45" s="11"/>
       <c r="J45" s="5"/>
@@ -5691,17 +5721,23 @@
         <v>787</v>
       </c>
       <c r="E46" s="11" t="s">
-        <v>19</v>
+        <v>574</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>110</v>
+        <v>331</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>851</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>853</v>
+      </c>
+      <c r="J46" s="5">
+        <v>1</v>
+      </c>
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
       <c r="M46" s="5"/>
@@ -5715,10 +5751,10 @@
         <v>787</v>
       </c>
       <c r="E47" s="11" t="s">
-        <v>19</v>
+        <v>574</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>2</v>
@@ -5736,20 +5772,18 @@
         <v>47</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>787</v>
+        <v>843</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>821</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>2</v>
-      </c>
+        <v>844</v>
+      </c>
+      <c r="F48" s="5">
+        <v>2</v>
+      </c>
+      <c r="G48" s="5"/>
       <c r="H48" s="11"/>
       <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
+      <c r="J48" s="5"/>
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
       <c r="M48" s="5"/>
@@ -5766,14 +5800,14 @@
         <v>19</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>2</v>
+        <v>111</v>
       </c>
       <c r="H49" s="11"/>
       <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
+      <c r="J49" s="5"/>
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
       <c r="M49" s="5"/>
@@ -5784,74 +5818,72 @@
         <v>49</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>840</v>
-      </c>
-      <c r="E50" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="E50" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>848</v>
-      </c>
-      <c r="I50" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H50" s="11"/>
+      <c r="I50" s="11"/>
       <c r="J50" s="5"/>
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
       <c r="M50" s="5"/>
-      <c r="N50" s="16"/>
+      <c r="N50" s="7"/>
     </row>
     <row r="51" spans="3:14">
       <c r="C51" s="5">
         <v>50</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>840</v>
-      </c>
-      <c r="E51" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="E51" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>116</v>
+        <v>821</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
+      <c r="H51" s="11"/>
+      <c r="I51" s="11"/>
+      <c r="J51" s="11"/>
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
       <c r="M51" s="5"/>
-      <c r="N51" s="16"/>
+      <c r="N51" s="7"/>
     </row>
     <row r="52" spans="3:14">
       <c r="C52" s="5">
         <v>51</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>840</v>
-      </c>
-      <c r="E52" s="5" t="s">
+        <v>787</v>
+      </c>
+      <c r="E52" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
-      <c r="J52" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="H52" s="11"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
       <c r="M52" s="5"/>
-      <c r="N52" s="16"/>
+      <c r="N52" s="7"/>
     </row>
     <row r="53" spans="3:14">
       <c r="C53" s="5">
@@ -5864,12 +5896,14 @@
         <v>19</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>111</v>
-      </c>
-      <c r="H53" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="H53" s="5" t="s">
+        <v>848</v>
+      </c>
       <c r="I53" s="5"/>
       <c r="J53" s="5"/>
       <c r="K53" s="5"/>
@@ -5888,20 +5922,14 @@
         <v>19</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" s="11" t="s">
-        <v>849</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>850</v>
-      </c>
-      <c r="J54" s="5" t="b">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
+      <c r="J54" s="5"/>
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
       <c r="M54" s="5"/>
@@ -5918,20 +5946,14 @@
         <v>19</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H55" s="5" t="s">
-        <v>851</v>
-      </c>
-      <c r="I55" s="5" t="s">
-        <v>850</v>
-      </c>
-      <c r="J55" s="5">
-        <v>2</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="H55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
       <c r="M55" s="5"/>
@@ -5951,7 +5973,7 @@
         <v>110</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -5961,88 +5983,102 @@
       <c r="M56" s="5"/>
       <c r="N56" s="16"/>
     </row>
-    <row r="57" spans="3:14" ht="15">
+    <row r="57" spans="3:14">
       <c r="C57" s="5">
         <v>56</v>
       </c>
-      <c r="D57" s="6" t="s">
-        <v>796</v>
-      </c>
-      <c r="E57" s="11"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="5"/>
-      <c r="J57" s="5"/>
+      <c r="D57" s="8" t="s">
+        <v>840</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>849</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="J57" s="5" t="b">
+        <v>1</v>
+      </c>
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
       <c r="M57" s="5"/>
-      <c r="N57" s="7"/>
+      <c r="N57" s="16"/>
     </row>
     <row r="58" spans="3:14">
       <c r="C58" s="5">
         <v>57</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>786</v>
-      </c>
-      <c r="E58" s="11" t="s">
-        <v>754</v>
-      </c>
-      <c r="F58" s="5">
-        <v>2</v>
-      </c>
-      <c r="G58" s="5"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="5"/>
-      <c r="J58" s="5"/>
+        <v>840</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>851</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>850</v>
+      </c>
+      <c r="J58" s="5">
+        <v>2</v>
+      </c>
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
       <c r="M58" s="5"/>
-      <c r="N58" s="7"/>
+      <c r="N58" s="16"/>
     </row>
     <row r="59" spans="3:14">
       <c r="C59" s="5">
         <v>58</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E59" s="11" t="s">
+        <v>840</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>19</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>22</v>
+        <v>110</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
       <c r="J59" s="5"/>
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
       <c r="M59" s="5"/>
-      <c r="N59" s="7"/>
+      <c r="N59" s="16"/>
     </row>
-    <row r="60" spans="3:14">
+    <row r="60" spans="3:14" ht="15">
       <c r="C60" s="5">
         <v>59</v>
       </c>
-      <c r="D60" s="8" t="s">
-        <v>787</v>
-      </c>
-      <c r="E60" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>2</v>
-      </c>
+      <c r="D60" s="6" t="s">
+        <v>796</v>
+      </c>
+      <c r="E60" s="11"/>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
       <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
+      <c r="I60" s="5"/>
       <c r="J60" s="5"/>
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
@@ -6054,74 +6090,70 @@
         <v>60</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>798</v>
+        <v>786</v>
       </c>
       <c r="E61" s="11" t="s">
-        <v>799</v>
-      </c>
-      <c r="F61" s="5" t="s">
-        <v>577</v>
-      </c>
-      <c r="G61" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="H61" s="5" t="s">
-        <v>800</v>
-      </c>
+        <v>754</v>
+      </c>
+      <c r="F61" s="5">
+        <v>2</v>
+      </c>
+      <c r="G61" s="5"/>
+      <c r="H61" s="11"/>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
       <c r="M61" s="5"/>
-      <c r="N61" s="16"/>
+      <c r="N61" s="7"/>
     </row>
-    <row r="62" spans="3:14" ht="14.25">
+    <row r="62" spans="3:14">
       <c r="C62" s="5">
         <v>61</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>798</v>
+        <v>787</v>
       </c>
       <c r="E62" s="11" t="s">
-        <v>799</v>
+        <v>19</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H62" s="17"/>
-      <c r="I62" s="5"/>
+      <c r="H62" s="11"/>
+      <c r="I62" s="11"/>
       <c r="J62" s="5"/>
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
       <c r="M62" s="5"/>
-      <c r="N62" s="16"/>
+      <c r="N62" s="7"/>
     </row>
     <row r="63" spans="3:14">
       <c r="C63" s="5">
         <v>62</v>
       </c>
       <c r="D63" s="8" t="s">
-        <v>798</v>
-      </c>
-      <c r="E63" s="5" t="s">
-        <v>583</v>
+        <v>787</v>
+      </c>
+      <c r="E63" s="11" t="s">
+        <v>19</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>203</v>
+        <v>74</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>2</v>
       </c>
       <c r="H63" s="11"/>
-      <c r="I63" s="5"/>
+      <c r="I63" s="11"/>
       <c r="J63" s="5"/>
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
       <c r="M63" s="5"/>
-      <c r="N63" s="16"/>
+      <c r="N63" s="7"/>
     </row>
     <row r="64" spans="3:14">
       <c r="C64" s="5">
@@ -6134,40 +6166,122 @@
         <v>799</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>95</v>
+        <v>577</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
+        <v>3</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>800</v>
+      </c>
+      <c r="I64" s="5"/>
       <c r="J64" s="5"/>
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
       <c r="M64" s="5"/>
-      <c r="N64" s="7"/>
+      <c r="N64" s="16"/>
+    </row>
+    <row r="65" spans="3:14" ht="14.25">
+      <c r="C65" s="5">
+        <v>64</v>
+      </c>
+      <c r="D65" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="E65" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H65" s="17"/>
+      <c r="I65" s="5"/>
+      <c r="J65" s="5"/>
+      <c r="K65" s="5"/>
+      <c r="L65" s="5"/>
+      <c r="M65" s="5"/>
+      <c r="N65" s="16"/>
+    </row>
+    <row r="66" spans="3:14">
+      <c r="C66" s="5">
+        <v>65</v>
+      </c>
+      <c r="D66" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>583</v>
+      </c>
+      <c r="F66" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H66" s="11"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
+      <c r="K66" s="5"/>
+      <c r="L66" s="5"/>
+      <c r="M66" s="5"/>
+      <c r="N66" s="16"/>
+    </row>
+    <row r="67" spans="3:14">
+      <c r="C67" s="5">
+        <v>66</v>
+      </c>
+      <c r="D67" s="8" t="s">
+        <v>798</v>
+      </c>
+      <c r="E67" s="11" t="s">
+        <v>799</v>
+      </c>
+      <c r="F67" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H67" s="11"/>
+      <c r="I67" s="11"/>
+      <c r="J67" s="5"/>
+      <c r="K67" s="5"/>
+      <c r="L67" s="5"/>
+      <c r="M67" s="5"/>
+      <c r="N67" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="N2:N64">
-    <cfRule type="cellIs" dxfId="1" priority="9" stopIfTrue="1" operator="equal">
+  <conditionalFormatting sqref="N2:N67">
+    <cfRule type="cellIs" dxfId="5" priority="11" stopIfTrue="1" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="10" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="12" stopIfTrue="1" operator="equal">
+      <formula>"Pass"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N8:N10">
+    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G62:G64 G2:G60">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G65:G67 G2:G63">
       <formula1>INDIRECT(SUBSTITUTE(E2&amp;F2," ",""))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D59:D60 D8:D18 D3:D4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D62:D63 D11:D21 D3:D4">
       <formula1>"C,F,T,;"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F9 F11:F67">
       <formula1>OFFSET(INDIRECT($E2),0,0,COUNTA(INDIRECT(E2&amp;"Col")),1)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E64">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E67">
       <formula1>Forms</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>